<commit_message>
updated excels with graphs
</commit_message>
<xml_diff>
--- a/results ex 3.xlsx
+++ b/results ex 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20202379\Documents\GitHub\Algorithms-for-Model-Checking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAC10B0-B4A3-4C3C-AEA6-A0044E0AE772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6620ADE-CEBE-49BC-98A4-95D476C73B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A8C04BDB-B96A-44B8-A47B-47C903334735}"/>
   </bookViews>
@@ -201,6 +201,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEB5600"/>
+      <color rgb="FF1A9988"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -314,7 +320,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:srgbClr val="1A9988"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -323,7 +329,71 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:delete val="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="144000" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -427,7 +497,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="EB5600"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -696,12 +766,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -779,26 +844,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -826,7 +871,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:srgbClr val="1A9988"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -878,10 +923,6 @@
                   <a:prstGeom prst="rect">
                     <a:avLst/>
                   </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
                 </c15:spPr>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -1003,7 +1044,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="EB5600"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1055,10 +1096,6 @@
                   <a:prstGeom prst="rect">
                     <a:avLst/>
                   </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
                 </c15:spPr>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -1336,12 +1373,574 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="1" i="1" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>player_2_can_win</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$B$1:$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Naïve algorithm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(Number of fixpoint iterations; e.g. 6)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="1A9988"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="144000" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>robots_50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>robots_100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>robots_150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>robots_200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>robots_250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>robots_300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>robots_350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>robots_400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>robots_450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>robots_500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>453</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>753</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>903</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1203</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1353</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1488-45CB-B90D-A0ECC0BB77C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$C$1:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>EL algorithm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(Number of fixpoint iterations; e.g. 6)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="EB5600"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>robots_50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>robots_100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>robots_150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>robots_200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>robots_250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>robots_300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>robots_350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>robots_400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>robots_450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>robots_500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$C$3:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>453</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>753</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>903</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1203</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1353</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1488-45CB-B90D-A0ECC0BB77C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1121563760"/>
+        <c:axId val="1121556080"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1121563760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1121556080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1121556080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1121563760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -2525,6 +3124,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>389408</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>21620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>82110</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>191595</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Grafiek 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67944A85-EF2D-4DCF-8578-B839D9F38001}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2852,8 +3489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88CDA0F3-4468-4A49-B0A0-3ED5D57F435D}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" zoomScale="104" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView tabSelected="1" topLeftCell="D12" zoomScale="106" zoomScaleNormal="104" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>